<commit_message>
Realizadas alterações na ordenação por data de criação mais recente dos ncms buscados nos métodos ncm-results ncm-results/export. Configurações finais no arquivo .env para resgate de variáveis de ambiente. Adicionado arquivo requirements para instalação do projeto em outras máquinas
</commit_message>
<xml_diff>
--- a/app/planilha.xlsx
+++ b/app/planilha.xlsx
@@ -917,7 +917,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -928,7 +928,7 @@
     <col width="38" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="36" customWidth="1" min="4" max="4"/>
+    <col width="129" customWidth="1" min="4" max="4"/>
     <col width="28" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -962,69 +962,188 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>22f1cc16-4929-4d7d-aacd-2485db653f79</t>
+          <t>0adac61f-b078-4812-86d4-af98abc9538f</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01.01</t>
+          <t>0102.3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CAVALOS, ASININOS E MUARES, VIVOS.</t>
+          <t>BÚFALOS:</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-20 16:08:05.834000</t>
+          <t>2025-05-21 10:56:42.301000</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>c1d3f1f1-0422-4883-a063-75d18b4d26d1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>8ed7eaf9-259f-4422-8a86-6bf706a844c6</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0102.29.11</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ANIMAIS VIVOS</t>
+          <t>Prenhes ou com cria ao pé</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-20 16:16:30.735000</t>
+          <t>2025-05-21 10:56:42.251000</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1f1a9dd4-39de-4a8d-abef-adc5c6366913</t>
+          <t>e1264496-3d8a-4650-8ee2-829419786d9e</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01.01</t>
+          <t>01.05</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CAVALOS, ASININOS E MUARES, VIVOS.</t>
+          <t>AVES DA ESPÉCIE GALLUS DOMESTICUS, PATOS, GANSOS, PERUS, PERUAS E GALINHAS-D’ANGOLA (PINTADAS), DAS ESPÉCIES DOMÉSTICAS, VIVOS.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-20 16:56:25.007000</t>
+          <t>2025-05-20 19:06:22.392000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3831aba8-4ff2-4c7c-859c-96789b1675c7</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01.05</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>AVES DA ESPÉCIE GALLUS DOMESTICUS, PATOS, GANSOS, PERUS, PERUAS E GALINHAS-D’ANGOLA (PINTADAS), DAS ESPÉCIES DOMÉSTICAS, VIVOS.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-05-20 18:57:28.911000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>f768e507-e1c8-4764-ad06-cfc6ff08999a</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0102.39.1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PARA REPRODUÇÃO</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-05-20 18:57:28.495000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>105f25df-4ffc-4487-b3bb-aae17a07d567</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0102.39.1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PARA REPRODUÇÃO</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-05-20 18:53:10.311000</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>e58092ef-e69a-47ec-9b6c-67245eac6716</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ANIMAIS VIVOS</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-05-20 18:41:05.422000</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>c1d3f1f1-0422-4883-a063-75d18b4d26d1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ANIMAIS VIVOS</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-05-20 16:16:30.735000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adição do fluxo completo de funcionalidades ao README
</commit_message>
<xml_diff>
--- a/app/planilha.xlsx
+++ b/app/planilha.xlsx
@@ -917,7 +917,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -928,7 +928,7 @@
     <col width="38" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="129" customWidth="1" min="4" max="4"/>
+    <col width="197" customWidth="1" min="4" max="4"/>
     <col width="28" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -962,186 +962,263 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0adac61f-b078-4812-86d4-af98abc9538f</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>30005f7a-2b93-4ab4-ba24-cebf5e09ff8c</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0102.3</t>
+          <t>0106.14.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BÚFALOS:</t>
+          <t>Coelhos e lebres</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-21 10:56:42.301000</t>
+          <t>2025-05-21 14:06:26.557000</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>8ed7eaf9-259f-4422-8a86-6bf706a844c6</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>NT</t>
-        </is>
-      </c>
+          <t>83c927d9-9d56-4428-82eb-f69cfdf448db</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0102.29.11</t>
+          <t>01.01</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Prenhes ou com cria ao pé</t>
+          <t>CAVALOS, ASININOS E MUARES, VIVOS.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-21 10:56:42.251000</t>
+          <t>2025-05-21 13:59:23.436000</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>e1264496-3d8a-4650-8ee2-829419786d9e</t>
+          <t>9b5af8eb-b5df-47bd-9cba-3d798003a9fd</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01.05</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>AVES DA ESPÉCIE GALLUS DOMESTICUS, PATOS, GANSOS, PERUS, PERUAS E GALINHAS-D’ANGOLA (PINTADAS), DAS ESPÉCIES DOMÉSTICAS, VIVOS.</t>
+          <t>ANIMAIS VIVOS</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-20 19:06:22.392000</t>
+          <t>2025-05-21 13:59:22.588000</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3831aba8-4ff2-4c7c-859c-96789b1675c7</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>911823be-8648-4824-89c1-ceb6e50a8666</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01.05</t>
+          <t>0106.12.00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>AVES DA ESPÉCIE GALLUS DOMESTICUS, PATOS, GANSOS, PERUS, PERUAS E GALINHAS-D’ANGOLA (PINTADAS), DAS ESPÉCIES DOMÉSTICAS, VIVOS.</t>
+          <t>Baleias, golfinhos e botos (mamíferos da ordem Cetacea); peixes-boi (manatins) e dugongos (mamíferos da ordem Sirenia); otárias e focas, leões-marinhos e morsas (mamíferos da subordem Pinnipedia)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-20 18:57:28.911000</t>
+          <t>2025-05-21 13:48:36.378000</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>f768e507-e1c8-4764-ad06-cfc6ff08999a</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
+          <t>4690ebbf-6196-4d85-848c-d50b750fe6cd</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NT</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0102.39.1</t>
+          <t>0105.12.00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PARA REPRODUÇÃO</t>
+          <t>Peruas e perus</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-20 18:57:28.495000</t>
+          <t>2025-05-21 13:48:35.319000</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>105f25df-4ffc-4487-b3bb-aae17a07d567</t>
+          <t>e1264496-3d8a-4650-8ee2-829419786d9e</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0102.39.1</t>
+          <t>01.05</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PARA REPRODUÇÃO</t>
+          <t>AVES DA ESPÉCIE GALLUS DOMESTICUS, PATOS, GANSOS, PERUS, PERUAS E GALINHAS-D’ANGOLA (PINTADAS), DAS ESPÉCIES DOMÉSTICAS, VIVOS.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-20 18:53:10.311000</t>
+          <t>2025-05-20 19:06:22.392000</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>e58092ef-e69a-47ec-9b6c-67245eac6716</t>
+          <t>3831aba8-4ff2-4c7c-859c-96789b1675c7</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>01.05</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ANIMAIS VIVOS</t>
+          <t>AVES DA ESPÉCIE GALLUS DOMESTICUS, PATOS, GANSOS, PERUS, PERUAS E GALINHAS-D’ANGOLA (PINTADAS), DAS ESPÉCIES DOMÉSTICAS, VIVOS.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-20 18:41:05.422000</t>
+          <t>2025-05-20 18:57:28.911000</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>c1d3f1f1-0422-4883-a063-75d18b4d26d1</t>
+          <t>f768e507-e1c8-4764-ad06-cfc6ff08999a</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
+          <t>0102.39.1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PARA REPRODUÇÃO</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-05-20 18:57:28.495000</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>105f25df-4ffc-4487-b3bb-aae17a07d567</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0102.39.1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PARA REPRODUÇÃO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-05-20 18:53:10.311000</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>e58092ef-e69a-47ec-9b6c-67245eac6716</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>ANIMAIS VIVOS</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-05-20 18:41:05.422000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>c1d3f1f1-0422-4883-a063-75d18b4d26d1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ANIMAIS VIVOS</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>2025-05-20 16:16:30.735000</t>
         </is>

</xml_diff>